<commit_message>
Sua Weekly_report_Crazy.xlsx va Weekly_Report_Son.xlsx
</commit_message>
<xml_diff>
--- a/BaoCaoNhom/Weekly_report_Crazy.xlsx
+++ b/BaoCaoNhom/Weekly_report_Crazy.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19440" windowHeight="9405"/>
+    <workbookView xWindow="390" yWindow="615" windowWidth="19440" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Project</t>
   </si>
@@ -436,15 +436,100 @@
   </si>
   <si>
     <t>Crazy</t>
+  </si>
+  <si>
+    <t>viết SRS ở các phần chung của nhóm (Mục đích tài liệu SRS, Yêu cầu môi trường hệ thống, Phát triển hệ thống, Định nghĩa các requirements)</t>
+  </si>
+  <si>
+    <t>1 phần SRS</t>
+  </si>
+  <si>
+    <t>90%, còn phải bổ sung các phần: Bảng viết tắt, Non-fuction requirements và detail non-function requirements</t>
+  </si>
+  <si>
+    <t>Viết SRS cho các function của cá nhân (bao gồm usecase và requirements của các chức năng: FAQ, Rule, Tìm kiếm sách, đăng ký mượn sách và hủy mượn sách)</t>
+  </si>
+  <si>
+    <t>Tổng hợp các phần của SRS thành báo cáo nhóm, gửi bài nộp lên sakai</t>
+  </si>
+  <si>
+    <t>SRS version 1.0</t>
+  </si>
+  <si>
+    <t>Hoàn chỉnh SRS cùng nhóm</t>
+  </si>
+  <si>
+    <t>SRS final</t>
+  </si>
+  <si>
+    <t>Viết SRS cho 4 chức năng Login/Logout, Register, Multlanguage và Profile</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
+  </si>
+  <si>
+    <t>Chụp hình usecase minh chứng cho 4 chức năng</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Quân</t>
+  </si>
+  <si>
+    <t>Đinh Trần Thái Sơn</t>
+  </si>
+  <si>
+    <t>Thiết lập SVN</t>
+  </si>
+  <si>
+    <t>Hoàn thành.</t>
+  </si>
+  <si>
+    <t>Vẽ lược đồ use case cho các chức năng: "Admin có thể xem thông tin mượn trả sách" và "Admin có thể xem thống kê về hoạt động mượn trả sách trong tuần/tháng"</t>
+  </si>
+  <si>
+    <t>Hoàn thành: xem lại lý thuyết về use case, cách vẽ; tham khảo các lược đồ của các thành viên khác trong nhóm để cách vẽ được đồng bộ.</t>
+  </si>
+  <si>
+    <t>Chỉnh lại một số chi tiết trong SRS</t>
+  </si>
+  <si>
+    <t>Hoàn thành: chỉnh "Admin" thành "Thủ thư" ở các chức năng 9 và 10.</t>
+  </si>
+  <si>
+    <t>Phạm Minh Thành</t>
+  </si>
+  <si>
+    <t>Viết SRS cho chức năng Send Mail và Thông tin mượn trả sách của người dùng</t>
+  </si>
+  <si>
+    <t>Chụp hình usecase minh chứng cho các chức năng trên</t>
+  </si>
+  <si>
+    <t>Đặng Ngọc Vũ</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Tổng hợp SRS version 1</t>
+  </si>
+  <si>
+    <t>SRS version 1</t>
+  </si>
+  <si>
+    <t>Tổng hợp report hàng tuần của nhóm</t>
+  </si>
+  <si>
+    <t>Report tuần 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -588,7 +673,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -615,6 +700,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3440,20 +3552,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="14" customWidth="1"/>
     <col min="2" max="3" width="16.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="10.75" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.875" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.125" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="6.25" style="3" customWidth="1"/>
     <col min="12" max="12" width="6" style="3" customWidth="1"/>
     <col min="13" max="13" width="5.875" style="3" customWidth="1"/>
@@ -3465,7 +3577,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3529,7 +3641,7 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -3554,7 +3666,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>27</v>
@@ -3569,61 +3681,117 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+    <row r="4" spans="1:30" ht="128.25">
+      <c r="A4" s="16">
+        <v>41171</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="10">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10">
+        <v>3</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+    <row r="5" spans="1:30" ht="142.5">
+      <c r="A5" s="16">
+        <v>41172</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="10">
+        <v>4</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:30">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+    <row r="6" spans="1:30" ht="57">
+      <c r="A6" s="12">
+        <v>41173</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+    <row r="7" spans="1:30" ht="28.5">
+      <c r="A7" s="9">
+        <v>41173</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>3</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -3643,143 +3811,261 @@
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
     </row>
-    <row r="8" spans="1:30">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+    <row r="8" spans="1:30" ht="57">
+      <c r="A8" s="16">
+        <v>41173</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:30">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+    <row r="9" spans="1:30" ht="71.25">
+      <c r="A9" s="16">
+        <v>41173</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:30">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:30" ht="57">
+      <c r="A10" s="16">
+        <v>41173</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="1:30" ht="57">
+      <c r="A11" s="16">
+        <v>41173</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:30">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+    <row r="12" spans="1:30" ht="71.25">
+      <c r="A12" s="16">
+        <v>41173</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+    <row r="13" spans="1:30" ht="57">
+      <c r="A13" s="12">
+        <v>41173</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+    <row r="14" spans="1:30" ht="28.5">
+      <c r="A14" s="9">
+        <v>41173</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.5</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+    <row r="15" spans="1:30" ht="28.5">
+      <c r="A15" s="9">
+        <v>41173</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>2</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+    <row r="16" spans="1:30" ht="42.75">
+      <c r="A16" s="16">
+        <v>41176</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10">
+        <v>8</v>
+      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="7"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3794,7 +4080,7 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="7"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -3809,7 +4095,7 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="7"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -3824,7 +4110,7 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="7"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -3839,7 +4125,7 @@
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="7"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -3854,7 +4140,7 @@
       <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="7"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -3869,7 +4155,7 @@
       <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="7"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -3884,7 +4170,7 @@
       <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="7"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -3899,6 +4185,10 @@
       <c r="M24" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A4:I16">
+    <sortCondition ref="A4:A16"/>
+    <sortCondition ref="I4:I16"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>

</xml_diff>